<commit_message>
aActualización al 08/04/2020 2
</commit_message>
<xml_diff>
--- a/3_inflacion_mensual.xlsx
+++ b/3_inflacion_mensual.xlsx
@@ -453,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B87"/>
+  <dimension ref="A1:B88"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="G83" sqref="G83"/>
+      <selection activeCell="F82" sqref="F82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1155,6 +1155,14 @@
       </c>
       <c r="B87" s="10">
         <v>22</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="8">
+        <v>43896</v>
+      </c>
+      <c r="B88" s="10">
+        <v>21.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>